<commit_message>
added product_code to schet-factura
</commit_message>
<xml_diff>
--- a/application/views/rpt/ua/doc/rakhunok_faktura.xlsx
+++ b/application/views/rpt/ua/doc/rakhunok_faktura.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\iSell\www\isell\application\views\rpt\ua\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="1596" yWindow="72" windowWidth="18192" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>№</t>
   </si>
@@ -109,6 +114,9 @@
   </si>
   <si>
     <t>{$v-&gt;rows[]-&gt;i}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_code}</t>
   </si>
 </sst>
 </file>
@@ -257,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -288,6 +296,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -316,13 +333,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -333,6 +344,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -381,7 +395,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,7 +430,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -625,240 +639,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C17"/>
+      <selection activeCell="A4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="54.42578125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.44140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="21" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-    </row>
-    <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="21" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="10" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="10" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="10" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="4"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="4"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="14" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="14" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -871,7 +908,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -883,7 +920,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>